<commit_message>
Creadas tablas de la base de datos
</commit_message>
<xml_diff>
--- a/bbdd.xlsx
+++ b/bbdd.xlsx
@@ -8,12 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\proyectoFinal-sipc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7EE136-2340-4136-B393-693BD0BA4B4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE386245-290D-4534-8ABE-194FA0DB08A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A366464D-F6C4-4283-BCF0-C66666764767}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="usuarios" sheetId="1" r:id="rId1"/>
+    <sheet name="mensajes_guia" sheetId="2" r:id="rId2"/>
+    <sheet name="guias" sheetId="3" r:id="rId3"/>
+    <sheet name="trofeos" sheetId="4" r:id="rId4"/>
+    <sheet name="comentarios_trofeos" sheetId="5" r:id="rId5"/>
+    <sheet name="foro" sheetId="6" r:id="rId6"/>
+    <sheet name="comentarios_foro" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>Nombre</t>
   </si>
@@ -186,10 +192,64 @@
     <t>Consejos para la primera partida:</t>
   </si>
   <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Donec dictum, enim ac auctor luctus, erat libero tempus mi, eu vulputate ligula sapien in ligula. Vestibulum viverra, ipsum ac convallis aliquam, nunc nunc eleifend tortor, id tincidunt lorem sapien finibus diam. Integer quis tortor aliquam lectus auctor convallis. Aenean facilisis felis ullamcorper nunc faucibus, nec posuere ante tincidunt. Phasellus nec purus ac massa elementum hendrerit non ac arcu. Ut elementum est in vestibulum sollicitudin. Proin at justo enim. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos. Ut eu purus quis ex cursus porta vel eu nibh. In aliquam mauris at varius iaculis. Nullam libero dolor, rutrum ac malesuada id, dignissim et odio. Etiam sit amet ex viverra, sagittis risus sed, viverra nulla. Ut quis lacus et orci ultrices viverra a nec enim.</t>
-  </si>
-  <si>
-    <t>Proin porta iaculis fringilla. Nam ligula dui, luctus sit amet mollis porttitor, tempor ut mi. Interdum et malesuada fames ac ante ipsum primis in faucibus. Mauris ornare non urna ut egestas. Cras lorem quam, varius vitae risus sodales, interdum vestibulum augue. Donec mattis ac nibh a placerat. Praesent non eros sit amet ante vulputate posuere. Nunc dui sapien, ornare nec fringilla sed, fringilla nec purus. Suspendisse ac elementum tortor. Nullam ullamcorper dolor eget sagittis malesuada. Integer elementum arcu enim, non tempor libero venenatis at. Donec finibus accumsan leo nec vehicula. Etiam tincidunt tempus lorem ut auctor. Phasellus quis viverra felis, et placerat dolor. Sed a neque velit. Integer at velit lobortis, pharetra mauris nec, suscipit diam.</t>
+    <t>Guía</t>
+  </si>
+  <si>
+    <t>id_juego</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>platino</t>
+  </si>
+  <si>
+    <t>¡enhorabuena!</t>
+  </si>
+  <si>
+    <t>Trofeos</t>
+  </si>
+  <si>
+    <t>id_trofeo</t>
+  </si>
+  <si>
+    <t>comentario</t>
+  </si>
+  <si>
+    <t>soy batman</t>
+  </si>
+  <si>
+    <t>conviértete en el murciélago</t>
+  </si>
+  <si>
+    <t>trofeo relacionado con la historia</t>
+  </si>
+  <si>
+    <t>comentarios_trofeos</t>
+  </si>
+  <si>
+    <t>fecha_creacion</t>
+  </si>
+  <si>
+    <t>hora_creacion</t>
+  </si>
+  <si>
+    <t>¿algún mod interesante para Skyrim?</t>
+  </si>
+  <si>
+    <t>Foro</t>
+  </si>
+  <si>
+    <t>id_foro</t>
+  </si>
+  <si>
+    <t>id_usuario</t>
+  </si>
+  <si>
+    <t>¿Alguien sabe de algún mod interesante? Es que llevo muchos años jugando a Skyrim y tengo ganas de cambiar un poco la trama original.</t>
+  </si>
+  <si>
+    <t>Comentarios del foro</t>
   </si>
 </sst>
 </file>
@@ -197,9 +257,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +279,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -260,11 +328,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -289,27 +354,83 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -628,284 +749,136 @@
   <dimension ref="B2:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="94.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="94.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="94.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" customWidth="1"/>
     <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="255.5703125" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>24948</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>36170</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="5">
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>36259</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="7">
-        <v>43828</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="4">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M15">
-        <v>3</v>
-      </c>
-      <c r="N15" t="s">
-        <v>46</v>
-      </c>
-      <c r="O15" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="Q16" t="s">
-        <v>51</v>
-      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="18" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="Q18" t="s">
-        <v>52</v>
-      </c>
+      <c r="Q18" s="35"/>
     </row>
     <row r="22" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F22" s="16"/>
+      <c r="F22" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B9:F9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{1CE2DC4A-A3CA-44AC-98D2-4EF9D7CB6C3D}"/>
@@ -915,4 +888,508 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D86917D-5E97-485A-885A-1CA8DF7B876C}">
+  <dimension ref="B2:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="94.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6">
+        <v>43828</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0230E883-08CE-4F48-8E97-5183B388F815}">
+  <dimension ref="B2:Q4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="36.42578125" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="22">
+        <v>0</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="22">
+        <v>7</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="20">
+        <v>0</v>
+      </c>
+      <c r="K4" s="20">
+        <v>0</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="20">
+        <v>3</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="20">
+        <v>61</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:Q2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C5A963-C917-47C6-A553-DAB50956FFCA}">
+  <dimension ref="B2:J28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+    </row>
+    <row r="3" spans="2:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="20">
+        <v>1</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="25"/>
+    </row>
+    <row r="17" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="25"/>
+    </row>
+    <row r="18" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0984F597-C599-4774-A78A-22E4408B68DB}">
+  <dimension ref="B2:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BE6C41-4F5E-421C-A895-A77E9BE83608}">
+  <dimension ref="B2:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="28"/>
+    <col min="3" max="3" width="34.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="22">
+        <v>0</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="32">
+        <v>43829</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0.83194444444444438</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0DC56A-360F-4CB2-804F-4C2AAAA12DE2}">
+  <dimension ref="B2:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B4" s="20">
+        <v>0</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0</v>
+      </c>
+      <c r="D4" s="20">
+        <v>0</v>
+      </c>
+      <c r="E4" s="32">
+        <v>43829</v>
+      </c>
+      <c r="F4" s="34">
+        <v>0.8340277777777777</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Realizado pequeño cambio en la estética de las tablas en Excel
</commit_message>
<xml_diff>
--- a/bbdd.xlsx
+++ b/bbdd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\proyectoFinal-sipc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE386245-290D-4534-8ABE-194FA0DB08A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2DE74F-51E8-4D7C-AC40-6DD8247A23D8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A366464D-F6C4-4283-BCF0-C66666764767}"/>
   </bookViews>
@@ -372,9 +372,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -403,34 +400,37 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -758,7 +758,7 @@
     <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="94.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" style="1" customWidth="1"/>
@@ -771,14 +771,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
@@ -871,7 +871,7 @@
       <c r="I6" s="12"/>
     </row>
     <row r="18" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="Q18" s="35"/>
+      <c r="Q18" s="31"/>
     </row>
     <row r="22" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F22" s="14"/>
@@ -908,13 +908,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -974,30 +974,30 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.7109375" customWidth="1"/>
-    <col min="15" max="15" width="36.42578125" style="18" customWidth="1"/>
+    <col min="15" max="15" width="36.42578125" style="17" customWidth="1"/>
     <col min="16" max="16" width="13.140625" customWidth="1"/>
     <col min="17" max="17" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1039,7 +1039,7 @@
       <c r="N3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="16" t="s">
         <v>32</v>
       </c>
       <c r="P3" s="5" t="s">
@@ -1049,53 +1049,53 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:17" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="22">
+    <row r="4" spans="2:17" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="21">
         <v>0</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <v>7</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="19">
         <v>0</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="19">
         <v>0</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="19">
         <v>3</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="O4" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="P4" s="20">
+      <c r="P4" s="19">
         <v>61</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="Q4" s="19" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1124,82 +1124,82 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-    </row>
-    <row r="3" spans="2:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+    </row>
+    <row r="3" spans="2:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+    <row r="4" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>0</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+    <row r="5" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="19">
         <v>1</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>1</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J16" s="25"/>
-    </row>
-    <row r="17" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J17" s="25"/>
-    </row>
-    <row r="18" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="10:10" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="24"/>
+    </row>
+    <row r="17" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="24"/>
+    </row>
+    <row r="18" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="10:10" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>
@@ -1222,31 +1222,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="16">
+      <c r="B4" s="15">
         <v>0</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>1</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1268,45 +1268,45 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="28"/>
-    <col min="3" max="3" width="34.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="25"/>
+    <col min="3" max="3" width="34.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="29" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="22">
+      <c r="B4" s="21">
         <v>0</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="28">
         <v>43829</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="29">
         <v>0.83194444444444438</v>
       </c>
     </row>
@@ -1328,61 +1328,61 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>0</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>0</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="19">
         <v>0</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="28">
         <v>43829</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="30">
         <v>0.8340277777777777</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="19" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>